<commit_message>
started working on the medication detail view UI
</commit_message>
<xml_diff>
--- a/MedbayTickets.xlsx
+++ b/MedbayTickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/universe-mac/Desktop/Medbay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B0C4501-6C56-1C4C-8587-E0AE7C421D2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDBA69E-92CC-524F-9032-6A884B3F3540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{3D1839B1-8D24-D049-8419-FDFD3A593D0E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Ticket #1</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Completed but can be improved</t>
+  </si>
+  <si>
+    <t>add images to camper object</t>
+  </si>
+  <si>
+    <t>Built medication detail view model</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +155,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -203,11 +215,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -217,8 +230,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +554,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,8 +562,8 @@
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="63.33203125" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
@@ -568,10 +586,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
@@ -580,10 +601,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="9"/>
       <c r="F3" t="s">
         <v>12</v>
       </c>
@@ -595,7 +616,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -603,7 +624,7 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -611,7 +632,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -624,61 +645,67 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="10"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E17" s="7"/>
+      <c r="E17" s="3"/>
       <c r="F17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E18" s="8"/>
+      <c r="E18" s="4"/>
       <c r="F18" t="s">
         <v>27</v>
       </c>

</xml_diff>